<commit_message>
minified import excel in product && productlogs
</commit_message>
<xml_diff>
--- a/public/uploads/sheetExcel/products.xlsx
+++ b/public/uploads/sheetExcel/products.xlsx
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">category_id  </t>
-  </si>
-  <si>
-    <t>brand_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>amount</t>
   </si>
@@ -80,6 +74,39 @@
   </si>
   <si>
     <t>كيلو</t>
+  </si>
+  <si>
+    <t>حماده  2</t>
+  </si>
+  <si>
+    <t>hamada 2</t>
+  </si>
+  <si>
+    <t>وصف  2</t>
+  </si>
+  <si>
+    <t>description 2</t>
+  </si>
+  <si>
+    <t>كيلو 2</t>
+  </si>
+  <si>
+    <t>kilo 2</t>
+  </si>
+  <si>
+    <t>برشام 2</t>
+  </si>
+  <si>
+    <t>kars 2</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>pharma</t>
+  </si>
+  <si>
+    <t>tram</t>
   </si>
 </sst>
 </file>
@@ -126,13 +153,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,149 +465,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="4"/>
-    <col min="5" max="5" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="3" width="9.140625" style="4"/>
+    <col min="4" max="4" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4">
         <v>20</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
+        <v>43963</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4">
         <v>20</v>
-      </c>
-      <c r="E2" s="3">
-        <v>43963</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
       </c>
       <c r="C3" s="4">
         <v>20</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
+        <v>43963</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3">
-        <v>43963</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>